<commit_message>
dummy data for analytical dataset
</commit_message>
<xml_diff>
--- a/i_codebooks/D4_analytical_dataset.xlsx
+++ b/i_codebooks/D4_analytical_dataset.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>medatata_name</t>
   </si>
@@ -173,9 +173,6 @@
     <t>binary</t>
   </si>
   <si>
-    <t>episode of bleeding (while in the source population), both 'broad' and 'narrow'</t>
-  </si>
-  <si>
     <t>1 = andexanet
 2a = andexanet precovid
 2b = andexanet covid
@@ -230,6 +227,12 @@
   </si>
   <si>
     <t>covariate_26</t>
+  </si>
+  <si>
+    <t>episode of bleeding (while in the source population)</t>
+  </si>
+  <si>
+    <t>whether the bleeding is identified with the 'narrow' strategy or with the 'possible' strategy</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -526,6 +529,9 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -854,7 +860,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -892,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="46.8">
@@ -944,16 +950,16 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="48" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="34.109375" style="3" customWidth="1"/>
@@ -1064,7 +1070,7 @@
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1083,7 @@
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1093,6 +1099,9 @@
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1102,105 +1111,105 @@
         <v>41</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="28.8">
       <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="28.8">
       <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="28.8">
       <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="28.8">
       <c r="A12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="28.8">
       <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="28.8">
       <c r="A14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="28.8">
       <c r="A15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1221,7 +1230,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>42</v>
@@ -1286,15 +1295,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dac44d48b4406d5c320fe911a853389">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="183e839aabd2ef2c305af4a754f6d8de" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -1539,6 +1539,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1552,14 +1561,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B7FC829-F037-49D5-9D9F-9F4592863FCD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1574,6 +1575,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>